<commit_message>
dos llamados, estado fisico funcional y ruta a imagen implementada
</commit_message>
<xml_diff>
--- a/reporte_imagenes.xlsx
+++ b/reporte_imagenes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="133">
   <si>
     <t>Latitud</t>
   </si>
@@ -52,13 +52,16 @@
     <t>Estado Físico</t>
   </si>
   <si>
+    <t>Ruta Imagen</t>
+  </si>
+  <si>
     <t>S20 39.4315</t>
   </si>
   <si>
     <t>S20 39.4604</t>
   </si>
   <si>
-    <t>S20 42.4067</t>
+    <t>S20 59.5334</t>
   </si>
   <si>
     <t>S20 59.5076</t>
@@ -67,7 +70,13 @@
     <t>S20 30.7616</t>
   </si>
   <si>
-    <t>S20 59.5334</t>
+    <t>S20 39.6866</t>
+  </si>
+  <si>
+    <t>S20 39.7412</t>
+  </si>
+  <si>
+    <t>S20 58.8237</t>
   </si>
   <si>
     <t>W68 43.0483</t>
@@ -76,7 +85,7 @@
     <t>W68 43.0293</t>
   </si>
   <si>
-    <t>W68 41.7026</t>
+    <t>W68 50.5161</t>
   </si>
   <si>
     <t>W68 50.5264</t>
@@ -85,34 +94,40 @@
     <t>W68 48.0732</t>
   </si>
   <si>
-    <t>W68 50.5161</t>
-  </si>
-  <si>
-    <t>W68 50.5063</t>
+    <t>W68 42.7603</t>
+  </si>
+  <si>
+    <t>W68 42.6934</t>
+  </si>
+  <si>
+    <t>W68 51.0752</t>
+  </si>
+  <si>
+    <t>3838 m</t>
+  </si>
+  <si>
+    <t>3840 M</t>
   </si>
   <si>
     <t>4355 m</t>
   </si>
   <si>
-    <t>3840 m</t>
-  </si>
-  <si>
-    <t>3811 m</t>
-  </si>
-  <si>
     <t>4354 m</t>
   </si>
   <si>
     <t>4296 m</t>
   </si>
   <si>
+    <t>3829 m</t>
+  </si>
+  <si>
     <t>4314 m</t>
   </si>
   <si>
     <t>4313 m</t>
   </si>
   <si>
-    <t>4310 m</t>
+    <t>4309 m</t>
   </si>
   <si>
     <t>4343 m</t>
@@ -133,6 +148,15 @@
     <t>102 km/h</t>
   </si>
   <si>
+    <t>92 km/h</t>
+  </si>
+  <si>
+    <t>36 km/h</t>
+  </si>
+  <si>
+    <t>90 km/h</t>
+  </si>
+  <si>
     <t>41 km/h</t>
   </si>
   <si>
@@ -160,13 +184,22 @@
     <t>2024/01/12 11:13:29</t>
   </si>
   <si>
+    <t>2024/01/12 11:28:30</t>
+  </si>
+  <si>
+    <t>2024/01/21 13:52:17</t>
+  </si>
+  <si>
+    <t>2024/01/12 11:28:36</t>
+  </si>
+  <si>
     <t>2024/01/21 13:54:21</t>
   </si>
   <si>
     <t>2024/01/21 13:54:27</t>
   </si>
   <si>
-    <t>2024/01/21 13:54:33</t>
+    <t>2024/01/21 13:54:34</t>
   </si>
   <si>
     <t>2024/01/21 13:52:19</t>
@@ -181,143 +214,212 @@
     <t>Pavimento asfáltico</t>
   </si>
   <si>
+    <t>Señalización_Vertical</t>
+  </si>
+  <si>
     <t>Alineamiento_Horizontal</t>
   </si>
   <si>
-    <t>Señalización_Horizontal</t>
-  </si>
-  <si>
-    <t>Señalización_Vertical</t>
-  </si>
-  <si>
     <t>Elementos_De_Contención_Vial</t>
   </si>
   <si>
-    <t>Se observan señales viales verticales de advertencia al lado derecho del camino, probablemente indicando una curva o giro en la carretera.</t>
-  </si>
-  <si>
-    <t>Se observa una señal de tránsito vertical que indica un límite de velocidad de 60 km/h. También hay una señal horizontal que indica el fin de la prohibición de adelantamiento.</t>
-  </si>
-  <si>
-    <t>Se observa una señal vertical de límite de velocidad de 50 km/h al costado de la carretera.</t>
+    <t>Sección_Transversal</t>
+  </si>
+  <si>
+    <t>Se observan varias señales de tránsito verticales a lo largo del camino, incluyendo una señal de advertencia amarilla que posiblemente indique una condición específica en la carretera más adelante.</t>
+  </si>
+  <si>
+    <t>Se observa una señal de tránsito vertical de indicación de fin de prohibición a la derecha del camino.</t>
+  </si>
+  <si>
+    <t>Se observa una señal de tránsito vertical de límite de velocidad a 50 km/h al costado del camino.</t>
   </si>
   <si>
     <t>Se observa una señal de tránsito vertical de advertencia, indicando un zigzag o serie de curvas adelante.</t>
   </si>
   <si>
-    <t>Se observa una señal de tránsito vertical de color azul ubicada a la orilla del camino que probablemente indica una ruta o dirección.</t>
-  </si>
-  <si>
-    <t>Se observa una señal de tránsito vertical que indica una advertencia, probablemente de un giro o curva en la carretera.</t>
-  </si>
-  <si>
-    <t>Se observa una señal de tránsito vertical de advertencia de curvas o giro en la carretera a lo lejos, a más de 5 metros de distancia.</t>
-  </si>
-  <si>
-    <t>Se observa una señal de tránsito vertical de color amarillo que indica un aviso, probablemente de alguna condición específica en la carretera.</t>
-  </si>
-  <si>
-    <t>Se observa una señal de tráfico vertical que indica una advertencia sobre una serie de curvas o zigzag más adelante en la ruta.</t>
-  </si>
-  <si>
-    <t>Se observa una señal de tránsito vertical al costado del camino que parece indicar una advertencia o información sobre alguna condición específica en la ruta.</t>
-  </si>
-  <si>
-    <t>No se observan eventos anormales o situaciones imprevistas en la ruta. El camino se encuentra despejado y sin presencia de trabajos, vehículos detenidos o animales.</t>
-  </si>
-  <si>
-    <t>No se observan eventos anormales o irregulares en la ruta. El camino se encuentra despejado y en buen estado.</t>
-  </si>
-  <si>
-    <t>No se observan eventos anormales en la ruta, el camino se encuentra despejado.</t>
+    <t>Se observa una señal vertical de color azul a la derecha del camino, pero no se puede identificar con claridad su contenido debido a la distancia.</t>
+  </si>
+  <si>
+    <t>Se observa una señal de tráfico vertical de advertencia de giro o curva peligrosa a la derecha ubicada a aproximadamente 50 metros del vehículo.</t>
+  </si>
+  <si>
+    <t>Se observa una señal de tránsito vertical de color amarillo que indica un aviso de 129 metros, probablemente refiriéndose a una condición específica en la carretera a esa distancia.</t>
+  </si>
+  <si>
+    <t>Se observa una señal de tránsito vertical a la derecha de la vía que indica una advertencia por una curva peligrosa o zigzag en el camino.</t>
+  </si>
+  <si>
+    <t>No se observan símbolos viales cercanos dentro de los 5 metros al costado del camino.</t>
+  </si>
+  <si>
+    <t>Se observa una señal de tránsito vertical de color amarillo que indica un aviso de advertencia a unos 129 metros, probablemente refiriéndose a una condición específica en la carretera a esa distancia.</t>
+  </si>
+  <si>
+    <t>Se observa una señal de tránsito vertical de color rojo que parece indicar una zona de trabajo o de precaución en la carretera.</t>
+  </si>
+  <si>
+    <t>No se observan eventos anormales o irregularidades en la ruta. El camino se encuentra despejado y en aparentes condiciones normales de tránsito.</t>
+  </si>
+  <si>
+    <t>No se observan eventos anormales en la ruta. El camino se encuentra despejado y en condiciones normales de tránsito.</t>
+  </si>
+  <si>
+    <t>No se observan eventos anormales en la ruta, el camino se encuentra despejado sin presencia de trabajos, vehículos detenidos o animales.</t>
   </si>
   <si>
     <t>No se observan eventos anormales en la ruta; el camino se encuentra despejado sin presencia de trabajos, vehículos detenidos, o animales.</t>
   </si>
   <si>
-    <t>No se observan eventos anormales en la ruta, el camino se encuentra despejado sin presencia de trabajos, vehículos detenidos o animales.</t>
-  </si>
-  <si>
-    <t>No se observan eventos anormales en el trayecto, la carretera se encuentra despejada y no hay presencia de trabajos, vehículos detenidos ni animales.</t>
-  </si>
-  <si>
-    <t>No se observan eventos anormales en la ruta; el camino se encuentra despejado sin presencia de trabajos, vehículos detenidos, ni animales.</t>
-  </si>
-  <si>
-    <t>No se observan eventos anormales o actividad inusual en la ruta según la imagen proporcionada.</t>
-  </si>
-  <si>
-    <t>La imagen muestra a una persona con equipo de seguridad trabajando en la vía, lo que sugiere posibles labores de mantenimiento o reparación en curso.</t>
-  </si>
-  <si>
-    <t>La carretera tiene una superficie de rodado de tipo granular, sin pavimento asfáltico ni de hormigón. Se aprecian algunas irregularidades y ondulaciones leves en la calzada, pero no se observan grandes hoyos o deterioros significativos.</t>
-  </si>
-  <si>
-    <t>La carretera tiene una superficie de rodado granular, sin presencia de pavimento asfáltico o de hormigón. El camino se encuentra nivelado y en buenas condiciones, sin grandes irregularidades ni hoyos visibles.</t>
-  </si>
-  <si>
-    <t>La carretera tiene una carpeta de rodado de tipo asfáltico, sin presencia de hoyos o irregularidades significativas. La superficie se encuentra en buen estado.</t>
+    <t>No se observan eventos anormales en la ruta, el camino se encuentra despejado y sin presencia de trabajos, vehículos detenidos o animales.</t>
+  </si>
+  <si>
+    <t>No se observan eventos anormales en la ruta. La carretera se encuentra despejada y en buenas condiciones para la circulación vehicular.</t>
+  </si>
+  <si>
+    <t>No se observan eventos anormales en la ruta en la imagen proporcionada.</t>
+  </si>
+  <si>
+    <t>No se observan eventos o condiciones anormales en la ruta, el camino se encuentra despejado y sin interrupciones.</t>
+  </si>
+  <si>
+    <t>No se observan eventos anormales en la ruta.</t>
+  </si>
+  <si>
+    <t>No se observan eventos anormales en la ruta; el camino está despejado y no hay presencia de personal de trabajo, vehículos detenidos, ni animales en la ruta.</t>
+  </si>
+  <si>
+    <t>Se observa a una persona trabajando en el camino, probablemente realizando labores de mantenimiento o reparación de la vía.</t>
+  </si>
+  <si>
+    <t>La carretera presenta una superficie de carpeta de rodado granular, sin pavimento asfáltico o de hormigón visible. Se observan algunas irregularidades menores en la superficie, pero no hay indicios de daños o deterioro severo.</t>
+  </si>
+  <si>
+    <t>La carpeta de rodado del camino es de tipo granular, sin presencia de pavimento asfáltico o de hormigón. La superficie se encuentra en buen estado, sin hoyos o irregularidades significativas visibles.</t>
+  </si>
+  <si>
+    <t>La carretera presenta una carpeta de rodado de pavimento asfáltico en buen estado, sin hoyos ni irregularidades significativas visibles.</t>
   </si>
   <si>
     <t>La calzada parece ser de carpeta de rodado tipo granular, en buenas condiciones y sin señales de deterioro significativo como hoyos o grandes irregularidades.</t>
   </si>
   <si>
-    <t>El camino presenta una carpeta de rodado de tipo granular, sin señales de pavimento asfáltico o de hormigón. La superficie se ve nivelada y sin presencia de grandes hoyos o irregularidades.</t>
-  </si>
-  <si>
-    <t>La carretera tiene una carpeta de rodado de tipo granular, sin pavimento asfáltico ni de hormigón. Se ven algunas leves irregularidades en la superficie, pero no se observan hoyos o deterioro significativo.</t>
-  </si>
-  <si>
-    <t>La carretera presenta una carpeta de rodado de tipo granular, sin pavimento asfáltico ni de hormigón visible. Hay algunas irregularidades leves en la superficie, pero en general se encuentra en un estado aceptable.</t>
-  </si>
-  <si>
-    <t>La calzada parece ser de carpeta de rodado tipo granular, en condiciones regulares con algunas irregularidades leves en la superficie. Hay presencia de barreras de contención a ambos lados del camino.</t>
-  </si>
-  <si>
-    <t>La carretera tiene una superficie de rodado de tipo granular, sin señales visibles de pavimento asfáltico o de hormigón. Hay algunas leves irregularidades en la superficie, pero no se aprecian hoyos, calaminas o piedras sueltas.</t>
-  </si>
-  <si>
-    <t>La carpeta de rodado parece ser de pavimento asfáltico, en aparente buen estado sin daños visibles.</t>
-  </si>
-  <si>
-    <t>El entorno está conformado por un paisaje árido y montañoso, con escasa vegetación. Se distinguen varias líneas de transmisión eléctrica que corren paralelas al trazado de la carretera, indicando la presencia de infraestructura eléctrica en la zona. No se observan otras estructuras u obras construidas en las cercanías.</t>
-  </si>
-  <si>
-    <t>El entorno muestra un paisaje desértico y montañoso, con vegetación escasa. Se observan postes y líneas de transmisión eléctrica a lo largo del camino, lo que indica una infraestructura de suministro de energía en la zona.</t>
-  </si>
-  <si>
-    <t>El entorno es predominantemente árido con vegetación escasa. Se observan montañas a lo lejos y postes de electricidad a lo largo de la ruta.</t>
+    <t>La carretera presenta una carpeta de rodado de tipo granular, sin señales de pavimento asfáltico o de hormigón. Se aprecian algunas irregularidades leves en la superficie, pero en general se encuentra en buen estado.</t>
+  </si>
+  <si>
+    <t>La calzada presenta una carpeta de rodado de pavimento asfáltico que se encuentra en buen estado, sin presencia de hoyos, grietas o irregularidades significativas. El camino muestra un alineamiento horizontal con una leve curva a la derecha.</t>
+  </si>
+  <si>
+    <t>La carretera tiene una carpeta de rodado de tipo granular, no hay presencia de pavimento y parece estar nivelada sin presencia de hoyos visibles. No hay señales de calaminas, piedras sueltas ni grandes irregularidades en la superficie.</t>
+  </si>
+  <si>
+    <t>La carretera presenta una carpeta de rodado de pavimento asfáltico en buen estado, sin presencia de hoyos, calaminas o irregularidades significativas en la superficie.</t>
+  </si>
+  <si>
+    <t>El camino muestra una superficie de rodado de tipo granular, sin presencia de pavimento asfáltico o de hormigón. Se aprecia una leve inclinación y curva en el trazado horizontal de la vía.</t>
+  </si>
+  <si>
+    <t>La superficie del camino es de tipo granular, sin pavimento asfáltico ni de hormigón. No se aprecian hoyos, irregularidades o deterioro significativo en la calzada.</t>
+  </si>
+  <si>
+    <t>Se observa una carretera con una carpeta de rodado granular, sin pavimento asfáltico ni de hormigón. Hay algunas irregularidades leves en la superficie y presencia de barreras de contención a ambos lados del camino.</t>
+  </si>
+  <si>
+    <t>La carretera tiene una carpeta de rodado de tipo asfáltico, parece estar en buenas condiciones y nivelada sin presencia de hoyos visibles. No hay señales de calaminas, piedras sueltas ni grandes irregularidades en la superficie.</t>
+  </si>
+  <si>
+    <t>La carretera en esta zona presenta una carpeta de rodado asfáltica en buen estado, sin presencia visible de irregularidades o deterioros significativos.</t>
+  </si>
+  <si>
+    <t>El entorno muestra un paisaje árido y montañoso, con poca vegetación a los lados de la carretera. Se distinguen postes y líneas de transmisión eléctrica que corren paralelos al camino, lo que sugiere la presencia de infraestructura eléctrica en la zona.</t>
+  </si>
+  <si>
+    <t>El entorno muestra un paisaje desértico con montañas en el fondo. No se observan estructuras construidas por el hombre además de los postes y líneas de transmisión eléctrica que acompañan el trazado de la carretera.</t>
+  </si>
+  <si>
+    <t>El entorno es un paisaje desértico con montañas al fondo, y se observan líneas de transmisión eléctrica paralelas al camino.</t>
   </si>
   <si>
     <t>El entorno consiste en un paisaje árido y montañoso con muy poca vegetación. No hay estructuras hechas por el hombre cerca de la carretera, con excepción de las señales de tránsito y los postes de electricidad visibles a lo largo de la ruta.</t>
   </si>
   <si>
-    <t>El entorno circundante muestra un paisaje árido, con escasa vegetación y montañas a lo lejos. No se observan estructuras hechas por el hombre más allá de la propia carretera, a excepción de algunos postes eléctricos distribuidos a lo largo del trayecto.</t>
-  </si>
-  <si>
-    <t>El entorno muestra un paisaje árido y montañoso, con poca vegetación. Se aprecian postes y líneas de transmisión eléctrica que recorren paralelos al camino, pero no hay otras estructuras o edificaciones visibles.</t>
-  </si>
-  <si>
-    <t>El entorno muestra un paisaje árido y montañoso, con vegetación escasa. Se observan postes y líneas de transmisión eléctrica paralelos a la carretera, lo que indica la presencia de infraestructura de energía en la zona.</t>
-  </si>
-  <si>
-    <t>El entorno consiste en un paisaje árido y montañoso con muy poca vegetación. Se observan postes de electricidad y líneas de transmisión eléctrica a lo largo de la ruta.</t>
-  </si>
-  <si>
-    <t>El entorno es principalmente de paisaje montañoso árido, con poca vegetación visible. Se observan postes y líneas de transmisión eléctrica que transcurren en paralelo a lo largo de la ruta, pero no hay otras estructuras o instalaciones evidentes.</t>
-  </si>
-  <si>
-    <t>El entorno muestra un paisaje montañoso con presencia de infraestructura eléctrica como torres y líneas de transmisión a lo largo de la carretera.</t>
+    <t>El entorno se caracteriza por un paisaje árido y montañoso, con poca vegetación circundante. No se observan estructuras hechas por el hombre, más allá de la infraestructura vial y los postes de energía eléctrica que se extienden a lo largo del camino.</t>
+  </si>
+  <si>
+    <t>El entorno es un paisaje desértico, con montañas en la distancia y poca vegetación. No se observan estructuras artificiales, más allá de la infraestructura vial como la señalización y postes eléctricos a lo largo de la ruta.</t>
+  </si>
+  <si>
+    <t>El entorno muestra una infraestructura de energía eléctrica con varios postes y líneas de transmisión distribuidas de manera regular a lo largo del paisaje. No se observan estructuras como casetas o torres diferentes a los postes de energía eléctrica ni tampoco presencia de agua o pozos visibles.</t>
+  </si>
+  <si>
+    <t>El entorno es un paisaje desértico, con montañas lejanas y algunas líneas de transmisión eléctrica paralelas a la carretera. No se observan estructuras, vehículos o personas fuera del vehículo en movimiento.</t>
+  </si>
+  <si>
+    <t>El entorno muestra un paisaje montañoso, árido y desértico, con muy poca vegetación. Además, se observa la presencia de postes y tendido eléctrico paralelos al camino, lo que indica una infraestructura de energía en la zona.</t>
+  </si>
+  <si>
+    <t>El entorno muestra un paisaje árido y montañoso, con poca vegetación. Se pueden ver postes y líneas eléctricas que corren paralelos a la carretera, lo que indica la presencia de infraestructura eléctrica en la zona.</t>
+  </si>
+  <si>
+    <t>El entorno comprende un paisaje árido con vegetación escasa, montañas en la distancia y presencia de líneas de transmisión eléctrica que siguen un trazado paralelo al camino, lo que sugiere una infraestructura de energía eléctrica.</t>
+  </si>
+  <si>
+    <t>El entorno muestra una infraestructura de energía eléctrica con varios postes y líneas de transmisión distribuidas de manera regular a lo largo del paisaje. No se observan otras estructuras hechas por el hombre ni presencia de agua o pozos visibles, solo un entorno montañoso árido.</t>
+  </si>
+  <si>
+    <t>El entorno muestra un paisaje árido con montañas a lo lejos y líneas de transmisión eléctrica que corren paralelas a la carretera, indicando la presencia de infraestructura eléctrica en la zona.</t>
   </si>
   <si>
     <t>Cumple</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_13652.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_15659.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_34151.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_36900.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_39902.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_41652.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_42401.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_47652.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_167150.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_172401.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_178401.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_44651.png</t>
+  </si>
+  <si>
+    <t>repo_imagenes\screenshot_7901.png</t>
+  </si>
+  <si>
+    <t>Ver Imagen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +434,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -366,16 +475,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,13 +783,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,393 +826,598 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L4" t="s">
+        <v>118</v>
+      </c>
+      <c r="M4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M5" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L6" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" t="s">
+        <v>123</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L2" t="s">
-        <v>98</v>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" t="s">
+        <v>118</v>
+      </c>
+      <c r="M7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K5" t="s">
-        <v>91</v>
-      </c>
-      <c r="L5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="L7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="K8" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="L8" t="s">
-        <v>98</v>
+        <v>118</v>
+      </c>
+      <c r="M8" t="s">
+        <v>125</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="K9" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="L9" t="s">
-        <v>98</v>
+        <v>118</v>
+      </c>
+      <c r="M9" t="s">
+        <v>126</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="K10" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="L10" t="s">
-        <v>98</v>
+        <v>118</v>
+      </c>
+      <c r="M10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" t="s">
+        <v>114</v>
+      </c>
+      <c r="L11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M11" t="s">
+        <v>128</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" t="s">
-        <v>96</v>
-      </c>
-      <c r="L11" t="s">
-        <v>98</v>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" t="s">
+        <v>115</v>
+      </c>
+      <c r="L12" t="s">
+        <v>118</v>
+      </c>
+      <c r="M12" t="s">
+        <v>129</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
         <v>42</v>
       </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" t="s">
         <v>87</v>
       </c>
-      <c r="K12" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" t="s">
-        <v>98</v>
+      <c r="J13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13" t="s">
+        <v>116</v>
+      </c>
+      <c r="L13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M13" t="s">
+        <v>130</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" t="s">
+        <v>118</v>
+      </c>
+      <c r="M14" t="s">
+        <v>131</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1"/>
+    <hyperlink ref="N3" r:id="rId2"/>
+    <hyperlink ref="N4" r:id="rId3"/>
+    <hyperlink ref="N5" r:id="rId4"/>
+    <hyperlink ref="N6" r:id="rId5"/>
+    <hyperlink ref="N7" r:id="rId6"/>
+    <hyperlink ref="N8" r:id="rId7"/>
+    <hyperlink ref="N9" r:id="rId8"/>
+    <hyperlink ref="N10" r:id="rId9"/>
+    <hyperlink ref="N11" r:id="rId10"/>
+    <hyperlink ref="N12" r:id="rId11"/>
+    <hyperlink ref="N13" r:id="rId12"/>
+    <hyperlink ref="N14" r:id="rId13"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>